<commit_message>
lavorato con MG per rivedere la pulizia dei dati. Ora passo a lei che esegue quanto detto sulle variabili SDO
</commit_message>
<xml_diff>
--- a/data/reparti.xlsx
+++ b/data/reparti.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanoorlando/Documents/RStudio/ica_cost/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanoorlando/Documents/RStudio/ica_cost2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46968E3-B02E-284E-898D-37C9F51AA616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF8DD5-6156-1C49-B384-642BA8227ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47520" yWindow="4740" windowWidth="31740" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>0906</t>
   </si>
   <si>
-    <t>UOSD  Chirurgia Maxillo facciale</t>
-  </si>
-  <si>
     <t>UOSD Dermatologia</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>reparto_cod</t>
+  </si>
+  <si>
+    <t>UOSD Chirurgia Maxillo facciale</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -935,10 +935,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -946,7 +946,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -954,23 +954,23 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -978,7 +978,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -994,7 +994,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1002,15 +1002,15 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1026,7 +1026,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1034,7 +1034,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1098,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1130,15 +1130,15 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1170,7 +1170,7 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1220,16 +1220,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1237,10 +1237,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="D2" s="10">
         <v>2677</v>
@@ -1251,10 +1251,10 @@
         <v>46</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="D3" s="10">
         <v>2677</v>
@@ -1268,7 +1268,7 @@
         <v>2477</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="10">
         <v>2477</v>
@@ -1282,7 +1282,7 @@
         <v>2673</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="10">
         <v>2677</v>
@@ -1296,7 +1296,7 @@
         <v>2674</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="10">
         <v>2677</v>
@@ -1310,7 +1310,7 @@
         <v>2675</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="10">
         <v>2677</v>
@@ -1324,7 +1324,7 @@
         <v>1977</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="10">
         <v>2677</v>
@@ -1338,7 +1338,7 @@
         <v>3275</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="10">
         <v>2677</v>
@@ -1352,7 +1352,7 @@
         <v>3276</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="10">
         <v>2677</v>
@@ -1366,7 +1366,7 @@
         <v>3675</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="10">
         <v>2677</v>
@@ -1380,7 +1380,7 @@
         <v>3676</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="10">
         <v>2677</v>
@@ -1394,7 +1394,7 @@
         <v>5077</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="10">
         <v>2677</v>
@@ -1408,7 +1408,7 @@
         <v>5877</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="10">
         <v>2677</v>
@@ -1422,7 +1422,7 @@
         <v>6877</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="10">
         <v>6877</v>
@@ -1436,7 +1436,7 @@
         <v>4974</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="10">
         <v>4977</v>
@@ -1450,7 +1450,7 @@
         <v>4975</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="10">
         <v>4977</v>
@@ -1464,7 +1464,7 @@
         <v>4976</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="10">
         <v>4977</v>
@@ -1478,7 +1478,7 @@
         <v>6674</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="11">
         <v>2677</v>
@@ -1492,7 +1492,7 @@
         <v>6675</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="11">
         <v>2677</v>
@@ -1506,7 +1506,7 @@
         <v>6676</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="11">
         <v>2677</v>
@@ -1520,7 +1520,7 @@
         <v>7177</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="11">
         <v>2677</v>
@@ -1531,10 +1531,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="D23" s="10">
         <v>2697</v>
@@ -1545,10 +1545,10 @@
         <v>46</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="D24" s="10">
         <v>2697</v>
@@ -1559,10 +1559,10 @@
         <v>41</v>
       </c>
       <c r="B25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="D25" s="16">
         <v>2497</v>
@@ -1576,7 +1576,7 @@
         <v>2693</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="10">
         <v>2697</v>
@@ -1590,7 +1590,7 @@
         <v>2694</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="10">
         <v>2697</v>
@@ -1604,7 +1604,7 @@
         <v>2695</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="10">
         <v>2697</v>
@@ -1618,7 +1618,7 @@
         <v>1997</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" s="10">
         <v>2697</v>
@@ -1632,7 +1632,7 @@
         <v>3295</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="10">
         <v>2697</v>
@@ -1646,7 +1646,7 @@
         <v>3296</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="10">
         <v>2697</v>
@@ -1660,7 +1660,7 @@
         <v>3695</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="10">
         <v>2697</v>
@@ -1674,7 +1674,7 @@
         <v>3696</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" s="10">
         <v>2697</v>
@@ -1685,10 +1685,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="D34" s="16">
         <v>2697</v>
@@ -1702,7 +1702,7 @@
         <v>5097</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" s="10">
         <v>2697</v>
@@ -1716,7 +1716,7 @@
         <v>5897</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="10">
         <v>2697</v>

</xml_diff>